<commit_message>
Corrected issue with Alexandra profile
When user doesn't supply any institutions, there is a weird error on their profile where it says "institution" and 'interests' where an actual affiliation should be. Corrected the profile.
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Alexandra_Clark/AlexandraClark_WebsiteForm.xlsx
+++ b/website_content_creation/authors/Alexandra_Clark/AlexandraClark_WebsiteForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Alexandra_Clark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{1CBF2EFD-9617-274A-B2FB-B0A561D4A127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5710A398-A5DC-4516-91F6-68AA1651CB20}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1CBF2EFD-9617-274A-B2FB-B0A561D4A127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1B437CE-57A6-407C-B23B-0949E2363786}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Watershed Ecology Team</t>
+  </si>
+  <si>
+    <t>glfc-wet.github.io</t>
   </si>
 </sst>
 </file>
@@ -562,9 +565,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -595,6 +595,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -813,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -847,7 +850,7 @@
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
@@ -866,7 +869,7 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>29</v>
       </c>
     </row>
@@ -880,18 +883,18 @@
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="32" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="7"/>
@@ -900,15 +903,15 @@
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="22"/>
       <c r="C12" t="s">
         <v>25</v>
       </c>
@@ -923,7 +926,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
@@ -939,20 +942,20 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="29" t="s">
         <v>14</v>
       </c>
     </row>
@@ -989,10 +992,10 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="41"/>
+      <c r="B24" s="40"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
@@ -1003,20 +1006,24 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="25"/>
+      <c r="A26" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24"/>
-      <c r="B27" s="27"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="26"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="24"/>
-      <c r="B28" s="27"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="26"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
-      <c r="B29" s="26"/>
+      <c r="B29" s="25"/>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
@@ -1032,27 +1039,27 @@
     </row>
     <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="25"/>
     </row>
     <row r="39" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>

</xml_diff>

<commit_message>
added a space to title for better visualization
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Alexandra_Clark/AlexandraClark_WebsiteForm.xlsx
+++ b/website_content_creation/authors/Alexandra_Clark/AlexandraClark_WebsiteForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Alexandra_Clark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{1CBF2EFD-9617-274A-B2FB-B0A561D4A127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B6AFE88-85AC-4F59-AC78-DB74F91301D3}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{1CBF2EFD-9617-274A-B2FB-B0A561D4A127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB767D3E-C695-42D3-B4FD-57EEDC0327DB}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,7 +154,7 @@
     <t>glfc-wet.github.io</t>
   </si>
   <si>
-    <t>Watershed Ecology Technician/Co-op Student</t>
+    <t>Watershed Ecology Technician/ Co-op Student</t>
   </si>
 </sst>
 </file>

</xml_diff>